<commit_message>
updated test data of protocols to have latest version of protocols data as base
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/18_protocols/test_data/test_update_dali.xlsx
+++ b/webcentral/doc/01_data/18_protocols/test_data/test_update_dali.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="248">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -203,9 +203,6 @@
     <t xml:space="preserve">Gebühr erforderlich</t>
   </si>
   <si>
-    <t xml:space="preserve">DALI_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.dali-alliance.org/</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t xml:space="preserve">Keine Gebühr erforderlich</t>
   </si>
   <si>
-    <t xml:space="preserve">Modbus_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.Modbus.org/</t>
   </si>
   <si>
@@ -293,9 +287,6 @@
     <t xml:space="preserve">Bitübertragungsschicht, Sicherungsschicht, Vermittlungsschicht, Anwendungsschicht</t>
   </si>
   <si>
-    <t xml:space="preserve">Zigbee_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://csa-iot.org/all-solutions/zigbee/</t>
   </si>
   <si>
@@ -329,9 +320,6 @@
     <t xml:space="preserve">Bitübertragungsschicht, Sicherungsschicht, Anwendungsschicht</t>
   </si>
   <si>
-    <t xml:space="preserve">EnOcean_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.enocean.com/de/</t>
   </si>
   <si>
@@ -359,9 +347,6 @@
     <t xml:space="preserve">Feldebene, Automationsebene, Managementebene</t>
   </si>
   <si>
-    <t xml:space="preserve">BACnet_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.bacnet.org/</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t xml:space="preserve">Gebühr erforderlich / offen (unklar)</t>
   </si>
   <si>
-    <t xml:space="preserve">profibus_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.profibus.com/technology/profibus/</t>
   </si>
   <si>
@@ -455,9 +437,6 @@
     <t xml:space="preserve">Transportschicht, Sitzungsschicht, Anwendungsschicht</t>
   </si>
   <si>
-    <t xml:space="preserve">OPC UA_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://opcfoundation.org/</t>
   </si>
   <si>
@@ -488,9 +467,6 @@
     <t xml:space="preserve">Bitübertragungsschicht, Sicherungsschicht, Vermittlungsschicht, Transportschicht, Anwendungsschicht</t>
   </si>
   <si>
-    <t xml:space="preserve">KNX_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.knx.org/</t>
   </si>
   <si>
@@ -518,9 +494,6 @@
     <t xml:space="preserve">Verwendet ein Prioritätsabfragemodell</t>
   </si>
   <si>
-    <t xml:space="preserve">LonWorks_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://www.lonmark.org/</t>
   </si>
   <si>
@@ -551,9 +524,6 @@
     <t xml:space="preserve">Data records</t>
   </si>
   <si>
-    <t xml:space="preserve">m-Bus_logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://m-bus.com/</t>
   </si>
   <si>
@@ -582,9 +552,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sicherungsschicht, Vermittlungsschicht, Anwendungsschicht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LoRaWan_logo.png</t>
   </si>
   <si>
     <t xml:space="preserve">https://lora-alliance.org/lorawan-for-developers/</t>
@@ -1106,7 +1073,7 @@
   <dimension ref="A1:AQ13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1294,108 +1261,104 @@
       <c r="T2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="W3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>53</v>
@@ -1404,10 +1367,10 @@
         <v>53</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>57</v>
@@ -1418,46 +1381,44 @@
       <c r="T4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="U4" s="2"/>
       <c r="V4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>54</v>
@@ -1466,10 +1427,10 @@
         <v>53</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>57</v>
@@ -1480,46 +1441,44 @@
       <c r="T5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="U5" s="2"/>
       <c r="V5" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>53</v>
@@ -1528,60 +1487,58 @@
         <v>53</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>58</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="U6" s="2"/>
       <c r="V6" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>54</v>
@@ -1590,60 +1547,60 @@
         <v>54</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>58</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>54</v>
@@ -1652,60 +1609,58 @@
         <v>53</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>53</v>
@@ -1714,13 +1669,13 @@
         <v>54</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>58</v>
@@ -1728,46 +1683,44 @@
       <c r="T9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U9" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="U9" s="2"/>
       <c r="V9" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>53</v>
@@ -1776,13 +1729,13 @@
         <v>53</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>58</v>
@@ -1790,46 +1743,44 @@
       <c r="T10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U10" s="2" t="s">
-        <v>155</v>
-      </c>
+      <c r="U10" s="2"/>
       <c r="V10" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>53</v>
@@ -1838,60 +1789,58 @@
         <v>53</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="2" t="s">
-        <v>165</v>
-      </c>
+      <c r="U11" s="2"/>
       <c r="V11" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>54</v>
@@ -1900,7 +1849,7 @@
         <v>54</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>57</v>
@@ -1909,48 +1858,46 @@
         <v>58</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="U12" s="2"/>
       <c r="V12" s="2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>54</v>
@@ -1959,7 +1906,7 @@
         <v>54</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>57</v>
@@ -1970,14 +1917,12 @@
       <c r="T13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U13" s="2" t="s">
-        <v>187</v>
-      </c>
+      <c r="U13" s="2"/>
       <c r="V13" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1998,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:AQ13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X12" activeCellId="0" sqref="X12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U15" activeCellId="0" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2069,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>22</v>
@@ -2140,10 +2085,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>46</v>
@@ -2152,13 +2097,13 @@
         <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>51</v>
@@ -2167,701 +2112,679 @@
         <v>52</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="W2" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="U3" s="2"/>
       <c r="V3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="K4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="W4" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="W5" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="L6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="W6" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="V7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="W7" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="W8" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="W9" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="U10" s="2"/>
+      <c r="V10" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="W10" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="W11" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="W12" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="M13" s="2" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="U13" s="2"/>
       <c r="V13" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>